<commit_message>
Change name from moonvale to moon, Fix bug of moonvale10.mp4 and Fix bug upload image, image changed
</commit_message>
<xml_diff>
--- a/excel/30_07_2025.xlsx
+++ b/excel/30_07_2025.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>18/12/2025</t>
+          <t>30/08/2025</t>
         </is>
       </c>
     </row>
@@ -498,12 +498,34 @@
       <c r="B7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n"/>
-      <c r="B8" s="1" t="n"/>
+      <c r="A8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Posted</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>01/08/2025</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
+      <c r="A9" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Posted</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10/08/2025</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -516,7 +538,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>08/12/2025</t>
+          <t>20/08/2025</t>
         </is>
       </c>
     </row>

</xml_diff>